<commit_message>
updated data model. Added empty route.
</commit_message>
<xml_diff>
--- a/LifePlanner/docs/data models.xlsx
+++ b/LifePlanner/docs/data models.xlsx
@@ -479,10 +479,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -696,7 +699,8 @@
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="80" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>